<commit_message>
updated fixture to latest version
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1604.10.rml.xlsx
+++ b/tests/fixtures/orderforms/1604.10.rml.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9515D7-FB80-AD4F-86F2-072E1240D92A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5AA305-0EF5-C94D-A9DB-7022C60A58EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DD23Ae9qJhC5962EjDbkniUmlV7E5os8o2LjlcGfzEUj5yt22g+hDV+kLwtoma25o0rM2RxA7HL+8jzO4x2tWA==" workbookSaltValue="3wB72j/MgB4sBrqBZE4epQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="3560" windowWidth="26220" windowHeight="17540" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="460" windowWidth="34580" windowHeight="17540" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orderform" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="968">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -3126,9 +3126,6 @@
     <t>FLUFFY</t>
   </si>
   <si>
-    <t xml:space="preserve">IDT DupSeq 10 bp Set B </t>
-  </si>
-  <si>
     <t>Removed index not in use any more</t>
   </si>
   <si>
@@ -3147,90 +3144,93 @@
     <t>Changed capture libray kit to sample concentration and the udf to UDF/Sample Conc.</t>
   </si>
   <si>
+    <t>IDT DupSeq 10 bp Set B</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>pool1</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>sample6</t>
+  </si>
+  <si>
+    <t>sample7</t>
+  </si>
+  <si>
+    <t>sample8</t>
+  </si>
+  <si>
     <t>pool2</t>
   </si>
   <si>
+    <t>sample9</t>
+  </si>
+  <si>
+    <t>sample10</t>
+  </si>
+  <si>
+    <t>sample11</t>
+  </si>
+  <si>
+    <t>sample12</t>
+  </si>
+  <si>
+    <t>sample13</t>
+  </si>
+  <si>
+    <t>sample14</t>
+  </si>
+  <si>
+    <t>sample15</t>
+  </si>
+  <si>
+    <t>sample16</t>
+  </si>
+  <si>
+    <t>sample17</t>
+  </si>
+  <si>
+    <t>missingpool</t>
+  </si>
+  <si>
+    <t>missingapptag</t>
+  </si>
+  <si>
+    <t>missingprio</t>
+  </si>
+  <si>
+    <t>missingvolume</t>
+  </si>
+  <si>
+    <t>missingconcentration</t>
+  </si>
+  <si>
+    <t>missingindex</t>
+  </si>
+  <si>
+    <t>missingindexnumber</t>
+  </si>
+  <si>
+    <t>missingpcontainername</t>
+  </si>
+  <si>
     <t>missingwell</t>
   </si>
   <si>
-    <t>missingpcontainername</t>
-  </si>
-  <si>
-    <t>missingindexnumber</t>
-  </si>
-  <si>
-    <t>missingindex</t>
-  </si>
-  <si>
-    <t>missingconcentration</t>
-  </si>
-  <si>
-    <t>missingvolume</t>
-  </si>
-  <si>
-    <t>missingprio</t>
-  </si>
-  <si>
-    <t>missingapptag</t>
-  </si>
-  <si>
-    <t>missingpool</t>
-  </si>
-  <si>
-    <t>sample17</t>
-  </si>
-  <si>
-    <t>sample16</t>
-  </si>
-  <si>
-    <t>sample15</t>
-  </si>
-  <si>
-    <t>sample14</t>
-  </si>
-  <si>
-    <t>sample13</t>
-  </si>
-  <si>
-    <t>sample12</t>
-  </si>
-  <si>
-    <t>sample11</t>
-  </si>
-  <si>
-    <t>sample10</t>
-  </si>
-  <si>
-    <t>sample9</t>
-  </si>
-  <si>
-    <t>sample8</t>
-  </si>
-  <si>
-    <t>pool1</t>
-  </si>
-  <si>
-    <t>sample7</t>
-  </si>
-  <si>
-    <t>sample6</t>
-  </si>
-  <si>
-    <t>sample5</t>
-  </si>
-  <si>
-    <t>sample4</t>
-  </si>
-  <si>
-    <t>sample3</t>
-  </si>
-  <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>sample1</t>
-  </si>
-  <si>
     <t>plate</t>
   </si>
   <si>
@@ -3238,6 +3238,72 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>pool3</t>
+  </si>
+  <si>
+    <t>pool4</t>
+  </si>
+  <si>
+    <t>pool5</t>
+  </si>
+  <si>
+    <t>pool6</t>
+  </si>
+  <si>
+    <t>pool7</t>
+  </si>
+  <si>
+    <t>pool8</t>
+  </si>
+  <si>
+    <t>pool9</t>
+  </si>
+  <si>
+    <t>pool10</t>
+  </si>
+  <si>
+    <t>pool11</t>
+  </si>
+  <si>
+    <t>pool12</t>
+  </si>
+  <si>
+    <t>pool13</t>
+  </si>
+  <si>
+    <t>pool14</t>
+  </si>
+  <si>
+    <t>pool15</t>
+  </si>
+  <si>
+    <t>pool16</t>
+  </si>
+  <si>
+    <t>pool17</t>
+  </si>
+  <si>
+    <t>pool18</t>
+  </si>
+  <si>
+    <t>pool19</t>
+  </si>
+  <si>
+    <t>pool20</t>
+  </si>
+  <si>
+    <t>pool21</t>
+  </si>
+  <si>
+    <t>pool22</t>
+  </si>
+  <si>
+    <t>pool23</t>
+  </si>
+  <si>
+    <t>pool24</t>
   </si>
 </sst>
 </file>
@@ -3248,7 +3314,7 @@
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="52" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3579,10 +3645,6 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="13">
@@ -4098,7 +4160,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4605,6 +4667,29 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="51" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="51" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4613,33 +4698,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="51" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="51" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="52" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="279">
@@ -5479,8 +5537,8 @@
   </sheetPr>
   <dimension ref="A1:Z399"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="124" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D5" zoomScale="124" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5737,23 +5795,23 @@
       <c r="Z8" s="149"/>
     </row>
     <row r="9" spans="1:26" s="152" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="187" t="s">
+      <c r="A9" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="188"/>
-      <c r="C9" s="188"/>
-      <c r="D9" s="188"/>
-      <c r="E9" s="188"/>
-      <c r="F9" s="188"/>
-      <c r="G9" s="188"/>
-      <c r="H9" s="188"/>
-      <c r="I9" s="188"/>
-      <c r="J9" s="189"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="194"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="194"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="194"/>
+      <c r="I9" s="194"/>
+      <c r="J9" s="195"/>
       <c r="K9" s="126"/>
-      <c r="L9" s="187" t="s">
+      <c r="L9" s="193" t="s">
         <v>102</v>
       </c>
-      <c r="M9" s="189"/>
+      <c r="M9" s="195"/>
       <c r="N9" s="126"/>
       <c r="O9" s="23" t="s">
         <v>82</v>
@@ -5763,10 +5821,10 @@
         <v>100</v>
       </c>
       <c r="R9" s="126"/>
-      <c r="S9" s="187" t="s">
+      <c r="S9" s="193" t="s">
         <v>334</v>
       </c>
-      <c r="T9" s="189"/>
+      <c r="T9" s="195"/>
       <c r="U9" s="134"/>
       <c r="V9" s="122"/>
       <c r="W9" s="151"/>
@@ -5855,7 +5913,7 @@
         <v>6</v>
       </c>
       <c r="T11" s="10" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="U11" s="153"/>
       <c r="W11" s="155"/>
@@ -5944,7 +6002,7 @@
         <v>76</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="U13" s="126"/>
       <c r="W13" s="164"/>
@@ -5982,13 +6040,13 @@
       <c r="Z14" s="167"/>
     </row>
     <row r="15" spans="1:26" s="170" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="194" t="s">
-        <v>942</v>
-      </c>
-      <c r="B15" s="191" t="s">
-        <v>935</v>
-      </c>
-      <c r="C15" s="193" t="s">
+      <c r="A15" s="187" t="s">
+        <v>915</v>
+      </c>
+      <c r="B15" s="188" t="s">
+        <v>919</v>
+      </c>
+      <c r="C15" s="189" t="s">
         <v>90</v>
       </c>
       <c r="D15" s="67" t="s">
@@ -6007,7 +6065,7 @@
         <v>2</v>
       </c>
       <c r="I15" s="65" t="s">
-        <v>908</v>
+        <v>914</v>
       </c>
       <c r="J15" s="65">
         <v>1</v>
@@ -6042,14 +6100,14 @@
       <c r="Z15" s="171"/>
     </row>
     <row r="16" spans="1:26" s="170" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="194" t="s">
-        <v>941</v>
-      </c>
-      <c r="B16" s="191" t="s">
-        <v>935</v>
-      </c>
-      <c r="C16" s="193" t="s">
-        <v>447</v>
+      <c r="A16" s="187" t="s">
+        <v>916</v>
+      </c>
+      <c r="B16" s="188" t="s">
+        <v>919</v>
+      </c>
+      <c r="C16" s="189" t="s">
+        <v>90</v>
       </c>
       <c r="D16" s="67" t="s">
         <v>446</v>
@@ -6096,14 +6154,14 @@
       <c r="Z16" s="171"/>
     </row>
     <row r="17" spans="1:26" s="170" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="194" t="s">
-        <v>940</v>
-      </c>
-      <c r="B17" s="191" t="s">
-        <v>935</v>
-      </c>
-      <c r="C17" s="193" t="s">
-        <v>448</v>
+      <c r="A17" s="187" t="s">
+        <v>917</v>
+      </c>
+      <c r="B17" s="188" t="s">
+        <v>924</v>
+      </c>
+      <c r="C17" s="189" t="s">
+        <v>447</v>
       </c>
       <c r="D17" s="67" t="s">
         <v>446</v>
@@ -6150,14 +6208,14 @@
       <c r="Z17" s="171"/>
     </row>
     <row r="18" spans="1:26" s="170" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="194" t="s">
-        <v>939</v>
-      </c>
-      <c r="B18" s="191" t="s">
-        <v>935</v>
-      </c>
-      <c r="C18" s="193" t="s">
-        <v>449</v>
+      <c r="A18" s="187" t="s">
+        <v>918</v>
+      </c>
+      <c r="B18" s="188" t="s">
+        <v>946</v>
+      </c>
+      <c r="C18" s="189" t="s">
+        <v>448</v>
       </c>
       <c r="D18" s="67" t="s">
         <v>446</v>
@@ -6204,14 +6262,14 @@
       <c r="Z18" s="171"/>
     </row>
     <row r="19" spans="1:26" s="170" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="194" t="s">
-        <v>938</v>
-      </c>
-      <c r="B19" s="196" t="s">
-        <v>935</v>
-      </c>
-      <c r="C19" s="193" t="s">
-        <v>450</v>
+      <c r="A19" s="187" t="s">
+        <v>920</v>
+      </c>
+      <c r="B19" s="188" t="s">
+        <v>947</v>
+      </c>
+      <c r="C19" s="189" t="s">
+        <v>449</v>
       </c>
       <c r="D19" s="67" t="s">
         <v>446</v>
@@ -6258,14 +6316,14 @@
       <c r="Z19" s="171"/>
     </row>
     <row r="20" spans="1:26" s="170" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="194" t="s">
-        <v>937</v>
-      </c>
-      <c r="B20" s="196" t="s">
-        <v>935</v>
-      </c>
-      <c r="C20" s="193" t="s">
-        <v>451</v>
+      <c r="A20" s="187" t="s">
+        <v>921</v>
+      </c>
+      <c r="B20" s="188" t="s">
+        <v>948</v>
+      </c>
+      <c r="C20" s="189" t="s">
+        <v>450</v>
       </c>
       <c r="D20" s="67" t="s">
         <v>446</v>
@@ -6312,14 +6370,14 @@
       <c r="Z20" s="171"/>
     </row>
     <row r="21" spans="1:26" s="170" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="194" t="s">
-        <v>936</v>
-      </c>
-      <c r="B21" s="196" t="s">
-        <v>935</v>
-      </c>
-      <c r="C21" s="193" t="s">
-        <v>452</v>
+      <c r="A21" s="187" t="s">
+        <v>922</v>
+      </c>
+      <c r="B21" s="188" t="s">
+        <v>949</v>
+      </c>
+      <c r="C21" s="189" t="s">
+        <v>451</v>
       </c>
       <c r="D21" s="67" t="s">
         <v>446</v>
@@ -6366,14 +6424,14 @@
       <c r="Z21" s="171"/>
     </row>
     <row r="22" spans="1:26" s="170" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="194" t="s">
-        <v>934</v>
-      </c>
-      <c r="B22" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C22" s="193" t="s">
-        <v>453</v>
+      <c r="A22" s="187" t="s">
+        <v>923</v>
+      </c>
+      <c r="B22" s="188" t="s">
+        <v>950</v>
+      </c>
+      <c r="C22" s="189" t="s">
+        <v>452</v>
       </c>
       <c r="D22" s="67" t="s">
         <v>446</v>
@@ -6422,14 +6480,14 @@
       <c r="Z22" s="171"/>
     </row>
     <row r="23" spans="1:26" s="172" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="194" t="s">
-        <v>933</v>
-      </c>
-      <c r="B23" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C23" s="193" t="s">
-        <v>454</v>
+      <c r="A23" s="187" t="s">
+        <v>925</v>
+      </c>
+      <c r="B23" s="188" t="s">
+        <v>951</v>
+      </c>
+      <c r="C23" s="189" t="s">
+        <v>453</v>
       </c>
       <c r="D23" s="67" t="s">
         <v>446</v>
@@ -6476,14 +6534,14 @@
       <c r="Z23" s="173"/>
     </row>
     <row r="24" spans="1:26" s="172" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="194" t="s">
-        <v>932</v>
-      </c>
-      <c r="B24" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C24" s="193" t="s">
-        <v>455</v>
+      <c r="A24" s="187" t="s">
+        <v>926</v>
+      </c>
+      <c r="B24" s="188" t="s">
+        <v>952</v>
+      </c>
+      <c r="C24" s="189" t="s">
+        <v>454</v>
       </c>
       <c r="D24" s="67" t="s">
         <v>446</v>
@@ -6530,14 +6588,14 @@
       <c r="Z24" s="173"/>
     </row>
     <row r="25" spans="1:26" s="172" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="194" t="s">
-        <v>931</v>
-      </c>
-      <c r="B25" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C25" s="193" t="s">
-        <v>456</v>
+      <c r="A25" s="187" t="s">
+        <v>927</v>
+      </c>
+      <c r="B25" s="188" t="s">
+        <v>953</v>
+      </c>
+      <c r="C25" s="189" t="s">
+        <v>455</v>
       </c>
       <c r="D25" s="67" t="s">
         <v>446</v>
@@ -6584,14 +6642,14 @@
       <c r="Z25" s="173"/>
     </row>
     <row r="26" spans="1:26" s="172" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="194" t="s">
-        <v>930</v>
-      </c>
-      <c r="B26" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C26" s="193" t="s">
-        <v>457</v>
+      <c r="A26" s="187" t="s">
+        <v>928</v>
+      </c>
+      <c r="B26" s="188" t="s">
+        <v>954</v>
+      </c>
+      <c r="C26" s="189" t="s">
+        <v>456</v>
       </c>
       <c r="D26" s="67" t="s">
         <v>446</v>
@@ -6638,14 +6696,14 @@
       <c r="Z26" s="173"/>
     </row>
     <row r="27" spans="1:26" s="174" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="194" t="s">
+      <c r="A27" s="187" t="s">
         <v>929</v>
       </c>
-      <c r="B27" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C27" s="190" t="s">
-        <v>463</v>
+      <c r="B27" s="188" t="s">
+        <v>955</v>
+      </c>
+      <c r="C27" s="189" t="s">
+        <v>457</v>
       </c>
       <c r="D27" s="67" t="s">
         <v>446</v>
@@ -6692,14 +6750,14 @@
       <c r="Z27" s="175"/>
     </row>
     <row r="28" spans="1:26" s="174" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="194" t="s">
-        <v>928</v>
-      </c>
-      <c r="B28" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C28" s="190" t="s">
-        <v>464</v>
+      <c r="A28" s="187" t="s">
+        <v>930</v>
+      </c>
+      <c r="B28" s="188" t="s">
+        <v>956</v>
+      </c>
+      <c r="C28" s="191" t="s">
+        <v>463</v>
       </c>
       <c r="D28" s="67" t="s">
         <v>446</v>
@@ -6746,14 +6804,14 @@
       <c r="Z28" s="175"/>
     </row>
     <row r="29" spans="1:26" s="174" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="194" t="s">
-        <v>927</v>
-      </c>
-      <c r="B29" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C29" s="190" t="s">
-        <v>465</v>
+      <c r="A29" s="187" t="s">
+        <v>931</v>
+      </c>
+      <c r="B29" s="188" t="s">
+        <v>957</v>
+      </c>
+      <c r="C29" s="191" t="s">
+        <v>464</v>
       </c>
       <c r="D29" s="67" t="s">
         <v>446</v>
@@ -6800,14 +6858,14 @@
       <c r="Z29" s="175"/>
     </row>
     <row r="30" spans="1:26" s="174" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="194" t="s">
-        <v>926</v>
-      </c>
-      <c r="B30" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C30" s="190" t="s">
-        <v>466</v>
+      <c r="A30" s="187" t="s">
+        <v>932</v>
+      </c>
+      <c r="B30" s="188" t="s">
+        <v>958</v>
+      </c>
+      <c r="C30" s="191" t="s">
+        <v>465</v>
       </c>
       <c r="D30" s="67" t="s">
         <v>446</v>
@@ -6854,14 +6912,14 @@
       <c r="Z30" s="175"/>
     </row>
     <row r="31" spans="1:26" s="174" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="194" t="s">
-        <v>925</v>
-      </c>
-      <c r="B31" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C31" s="190" t="s">
-        <v>467</v>
+      <c r="A31" s="187" t="s">
+        <v>933</v>
+      </c>
+      <c r="B31" s="188" t="s">
+        <v>959</v>
+      </c>
+      <c r="C31" s="191" t="s">
+        <v>466</v>
       </c>
       <c r="D31" s="67" t="s">
         <v>446</v>
@@ -6908,12 +6966,12 @@
       <c r="Z31" s="175"/>
     </row>
     <row r="32" spans="1:26" s="174" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="194" t="s">
-        <v>924</v>
-      </c>
-      <c r="B32" s="191"/>
-      <c r="C32" s="190" t="s">
-        <v>468</v>
+      <c r="A32" s="187" t="s">
+        <v>934</v>
+      </c>
+      <c r="B32" s="188"/>
+      <c r="C32" s="191" t="s">
+        <v>467</v>
       </c>
       <c r="D32" s="67" t="s">
         <v>446</v>
@@ -6960,13 +7018,13 @@
       <c r="Z32" s="175"/>
     </row>
     <row r="33" spans="1:26" s="174" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="194" t="s">
-        <v>923</v>
-      </c>
-      <c r="B33" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C33" s="195"/>
+      <c r="A33" s="187" t="s">
+        <v>935</v>
+      </c>
+      <c r="B33" s="188" t="s">
+        <v>960</v>
+      </c>
+      <c r="C33" s="190"/>
       <c r="D33" s="67" t="s">
         <v>446</v>
       </c>
@@ -7012,18 +7070,16 @@
       <c r="Z33" s="175"/>
     </row>
     <row r="34" spans="1:26" s="174" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="194" t="s">
-        <v>922</v>
-      </c>
-      <c r="B34" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C34" s="190" t="s">
-        <v>469</v>
-      </c>
-      <c r="D34" s="67" t="s">
-        <v>446</v>
-      </c>
+      <c r="A34" s="187" t="s">
+        <v>936</v>
+      </c>
+      <c r="B34" s="188" t="s">
+        <v>961</v>
+      </c>
+      <c r="C34" s="191" t="s">
+        <v>468</v>
+      </c>
+      <c r="D34" s="67"/>
       <c r="E34" s="63" t="s">
         <v>907</v>
       </c>
@@ -7066,14 +7122,14 @@
       <c r="Z34" s="175"/>
     </row>
     <row r="35" spans="1:26" s="174" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="194" t="s">
-        <v>921</v>
-      </c>
-      <c r="B35" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C35" s="190" t="s">
-        <v>470</v>
+      <c r="A35" s="187" t="s">
+        <v>937</v>
+      </c>
+      <c r="B35" s="188" t="s">
+        <v>962</v>
+      </c>
+      <c r="C35" s="191" t="s">
+        <v>469</v>
       </c>
       <c r="D35" s="67" t="s">
         <v>446</v>
@@ -7084,7 +7140,7 @@
       <c r="F35" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="195"/>
+      <c r="G35" s="190"/>
       <c r="H35" s="65">
         <v>2</v>
       </c>
@@ -7118,14 +7174,14 @@
       <c r="Z35" s="175"/>
     </row>
     <row r="36" spans="1:26" s="176" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="194" t="s">
-        <v>920</v>
-      </c>
-      <c r="B36" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C36" s="190" t="s">
-        <v>471</v>
+      <c r="A36" s="187" t="s">
+        <v>938</v>
+      </c>
+      <c r="B36" s="188" t="s">
+        <v>963</v>
+      </c>
+      <c r="C36" s="191" t="s">
+        <v>470</v>
       </c>
       <c r="D36" s="67" t="s">
         <v>446</v>
@@ -7170,14 +7226,14 @@
       <c r="Z36" s="177"/>
     </row>
     <row r="37" spans="1:26" s="176" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="194" t="s">
-        <v>919</v>
-      </c>
-      <c r="B37" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C37" s="193" t="s">
-        <v>458</v>
+      <c r="A37" s="187" t="s">
+        <v>939</v>
+      </c>
+      <c r="B37" s="188" t="s">
+        <v>964</v>
+      </c>
+      <c r="C37" s="191" t="s">
+        <v>471</v>
       </c>
       <c r="D37" s="67" t="s">
         <v>446</v>
@@ -7222,14 +7278,14 @@
       <c r="Z37" s="177"/>
     </row>
     <row r="38" spans="1:26" s="176" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="194" t="s">
-        <v>918</v>
-      </c>
-      <c r="B38" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C38" s="193" t="s">
-        <v>459</v>
+      <c r="A38" s="187" t="s">
+        <v>940</v>
+      </c>
+      <c r="B38" s="188" t="s">
+        <v>965</v>
+      </c>
+      <c r="C38" s="189" t="s">
+        <v>458</v>
       </c>
       <c r="D38" s="67" t="s">
         <v>446</v>
@@ -7275,13 +7331,13 @@
     </row>
     <row r="39" spans="1:26" s="172" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="192" t="s">
-        <v>917</v>
-      </c>
-      <c r="B39" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C39" s="190" t="s">
-        <v>899</v>
+        <v>941</v>
+      </c>
+      <c r="B39" s="188" t="s">
+        <v>966</v>
+      </c>
+      <c r="C39" s="189" t="s">
+        <v>459</v>
       </c>
       <c r="D39" s="67" t="s">
         <v>446</v>
@@ -7327,12 +7383,12 @@
     </row>
     <row r="40" spans="1:26" s="172" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="118" t="s">
-        <v>916</v>
-      </c>
-      <c r="B40" s="191" t="s">
-        <v>915</v>
-      </c>
-      <c r="C40" s="190" t="s">
+        <v>942</v>
+      </c>
+      <c r="B40" s="188" t="s">
+        <v>967</v>
+      </c>
+      <c r="C40" s="191" t="s">
         <v>899</v>
       </c>
       <c r="D40" s="67" t="s">
@@ -18164,12 +18220,6 @@
           </x14:formula1>
           <xm:sqref>D16:D398</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E4ADDAE-168B-A04D-8345-0235D21293BD}">
-          <x14:formula1>
-            <xm:f>'Drop down list'!$H$1:$H$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>C15:C398</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{61A33616-F508-0D43-A142-E2FCF2C85494}">
           <x14:formula1>
             <xm:f>'Drop down list'!$F$1:$F$300</xm:f>
@@ -18206,6 +18256,12 @@
           </x14:formula1>
           <xm:sqref>I15</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E4ADDAE-168B-A04D-8345-0235D21293BD}">
+          <x14:formula1>
+            <xm:f>'Drop down list'!$H$1:$H$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>C34:C398 C16:C32</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -18328,22 +18384,22 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="185" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="185" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="185" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="185" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.15">
@@ -18593,7 +18649,7 @@
   <dimension ref="A1:L396"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H24" sqref="H1:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -22369,7 +22425,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="AFA6uq6/dwRSvb0ZQ4czYU8/0k2fNGAxUioIBV8iDSPMOsLTom7BZPbPux0y8zLId2p3q2sjXzEAATfu0Tozaw==" saltValue="chER4y0CMsNH3dg6NLbRfA==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -22386,7 +22442,7 @@
   <dimension ref="A1:N386"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -22435,7 +22491,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>908</v>
+        <v>914</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>89</v>
@@ -22455,7 +22511,7 @@
     </row>
     <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>908</v>
+        <v>914</v>
       </c>
       <c r="B3" s="33">
         <v>1</v>
@@ -30797,7 +30853,7 @@
       <c r="M386" s="31"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="CSevnaEGTT/q32bGyb4Heovok3J5PX5+lnPjhwrYN1Y6X73Z3KDcEUZb/QJAY4LiVO3hGxPr5QDpJ9rYayTn7A==" saltValue="H/jxIXY7qZtcce4fkLPuhw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>